<commit_message>
Sæt baggrundsfarve på tests
</commit_message>
<xml_diff>
--- a/05 Test/STD0101 angivBruttofortjenesteOgVareforbrug.xlsx
+++ b/05 Test/STD0101 angivBruttofortjenesteOgVareforbrug.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tommy\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tommy\Desktop\ændringer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B90ECD5A-3237-421E-8F9D-617244908825}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FAE3FF2-87A6-455B-83C0-DF7542ADA223}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{289DCCEB-661B-43E8-8E46-F3BB1C33AEE6}"/>
+    <workbookView xWindow="1884" yWindow="1884" windowWidth="17280" windowHeight="8964" xr2:uid="{289DCCEB-661B-43E8-8E46-F3BB1C33AEE6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -84,12 +84,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -104,9 +110,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,7 +431,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -449,73 +456,84 @@
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>12698</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="2">
         <v>34320</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>21622</v>
       </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>-2698</v>
       </c>
-      <c r="E5" t="s">
+      <c r="D5" s="2"/>
+      <c r="E5" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <v>21622</v>
       </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="2">
         <v>12698</v>
       </c>
-      <c r="E8" t="s">
+      <c r="D8" s="2"/>
+      <c r="E8" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="2">
         <v>-1622</v>
       </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>